<commit_message>
Adjusted testdata for TC verifyGetStartedPages
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeanlexterserra/IdeaProjects/SGBBAPPAutomation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ADB1F8-8989-184C-A07B-A9EC6734FF19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9C54B2-24B2-644F-BE0A-50B1511A4276}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7180" yWindow="-22380" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="-14520" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testdata" sheetId="4" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>IOS Locator</t>
   </si>
   <si>
-    <t>loginUser1</t>
-  </si>
-  <si>
     <t>btnGetStarted</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   <si>
     <t>text1=Welcome
 to Globe myBusiness</t>
+  </si>
+  <si>
+    <t>verifyGetStartedPages</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -487,19 +487,19 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -548,7 +548,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -557,36 +557,36 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>